<commit_message>
changed some spreadsheet stuff
</commit_message>
<xml_diff>
--- a/NTC2_-_Compact_Crafting_Recipe_Book.xlsx
+++ b/NTC2_-_Compact_Crafting_Recipe_Book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MLefebvre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MLefebvre\curseforge\minecraft\Instances\1.16.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FB66D9-CDD4-462F-90DD-94E108D85C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB44954-21A3-4FC5-B037-DD95084E3310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{8AC89A7E-C86E-4B90-A23B-0FA9309DBAB4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="80">
   <si>
     <t>Quantum Ring</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Calculation Processor</t>
   </si>
   <si>
-    <t>Printed Silicon</t>
-  </si>
-  <si>
     <t>16k Storage Component</t>
   </si>
   <si>
@@ -255,6 +252,33 @@
   </si>
   <si>
     <t>16M Storage Component</t>
+  </si>
+  <si>
+    <t>Charged Certus Quartz</t>
+  </si>
+  <si>
+    <t>Using the LazierAe2 Etcher</t>
+  </si>
+  <si>
+    <t>Purified Certus Quartz</t>
+  </si>
+  <si>
+    <t>Total Redstone Dust</t>
+  </si>
+  <si>
+    <t>Total Silicon</t>
+  </si>
+  <si>
+    <t>Total Sand</t>
+  </si>
+  <si>
+    <t>Certus Quartz Dust</t>
+  </si>
+  <si>
+    <t>Total Certus Quartz Dust</t>
+  </si>
+  <si>
+    <t>Total Glowstone</t>
   </si>
 </sst>
 </file>
@@ -266,7 +290,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +335,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,8 +368,18 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -535,14 +584,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -577,26 +641,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="1" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
@@ -967,12 +1039,12 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1062,20 +1134,20 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1384,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52F51F3-3F78-4BDC-A353-26EDF8D65C66}">
   <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,13 +2273,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="7:11" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
@@ -2290,570 +2362,1209 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C382D8E-1217-4973-B5EA-3A96266568D3}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection sqref="A1:P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="36"/>
+    <col min="1" max="1" width="24.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" style="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="36">
-        <f>1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="B1" s="39">
+        <v>360000</v>
+      </c>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="40">
+        <f>B4+H5+J9+J14+J19+J24+J29+J34+J39+D8+D23+D28</f>
+        <v>5431680000</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="40">
+        <f>J5+H10+H15+H20+H25+H30+H35+H40</f>
+        <v>1180800000</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="40">
+        <f>D10+D15+D20+D25+D30+D35+D40</f>
+        <v>393480000</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="40">
+        <f>B9+B14+B19+B24+B29+B34+B39</f>
+        <v>491850000</v>
+      </c>
+      <c r="O1" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="40">
+        <f>D13+D18+D33+D38</f>
+        <v>472320000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="39">
         <f>F8</f>
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+        <v>787320000</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="39">
         <f>B3*4</f>
-        <v>8748</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="36">
+        <v>3149280000</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="39">
         <f>B3*4</f>
-        <v>8748</v>
-      </c>
-      <c r="E4" s="37" t="s">
+        <v>3149280000</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="42">
         <f>B3*1</f>
-        <v>2187</v>
-      </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E5" s="40" t="s">
+        <v>787320000</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="45">
         <f>F4*1</f>
-        <v>2187</v>
-      </c>
-      <c r="G5" s="42" t="s">
+        <v>787320000</v>
+      </c>
+      <c r="G5" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="45">
         <f>F4*1</f>
-        <v>2187</v>
-      </c>
-      <c r="I5" s="42" t="s">
+        <v>787320000</v>
+      </c>
+      <c r="I5" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="47">
         <f>F4*1</f>
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+        <v>787320000</v>
+      </c>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="39">
         <f>F13</f>
-        <v>729</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+        <v>262440000</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="39">
         <f>B7*1</f>
-        <v>729</v>
-      </c>
-      <c r="C8" s="36" t="s">
+        <v>262440000</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="39">
         <f>B7*4</f>
-        <v>2916</v>
-      </c>
-      <c r="E8" s="36" t="s">
+        <v>1049760000</v>
+      </c>
+      <c r="E8" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="39">
         <f>B7*3</f>
-        <v>2187</v>
-      </c>
-      <c r="G8" s="37" t="s">
+        <v>787320000</v>
+      </c>
+      <c r="G8" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="42">
         <f>B7*1</f>
-        <v>729</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G9" s="44" t="s">
+        <v>262440000</v>
+      </c>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="42">
+        <f>5/4*B8</f>
+        <v>328050000</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="43">
+        <f>4/4*B8</f>
+        <v>262440000</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="51">
+        <f>H8*1</f>
+        <v>262440000</v>
+      </c>
+      <c r="I9" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="52">
+        <f>H8*1</f>
+        <v>262440000</v>
+      </c>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="53"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="47">
+        <f>1*D9</f>
+        <v>262440000</v>
+      </c>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="45">
+        <f>H9*1</f>
+        <v>262440000</v>
+      </c>
+      <c r="I10" s="45"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="45">
-        <f>H8*1</f>
-        <v>729</v>
-      </c>
-      <c r="I9" s="46" t="s">
+      <c r="B12" s="51">
+        <f>F18</f>
+        <v>87480000</v>
+      </c>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="51">
+        <f>B12*1</f>
+        <v>87480000</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="51">
+        <f>B12*4</f>
+        <v>349920000</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="39">
+        <f>B12*3</f>
+        <v>262440000</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="42">
+        <f>B12*1</f>
+        <v>87480000</v>
+      </c>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="42">
+        <f>5/4*B13</f>
+        <v>109350000</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="43">
+        <f>4/4*B13</f>
+        <v>87480000</v>
+      </c>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="51">
+        <f>H13*1</f>
+        <v>87480000</v>
+      </c>
+      <c r="I14" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="47">
-        <f>H8*1</f>
-        <v>729</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G10" s="40" t="s">
+      <c r="J14" s="52">
+        <f>H13*1</f>
+        <v>87480000</v>
+      </c>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="53"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="47">
+        <f>1*D14</f>
+        <v>87480000</v>
+      </c>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="41">
-        <f>H9*1</f>
-        <v>729</v>
-      </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="43"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="H15" s="45">
+        <f>H14*1</f>
+        <v>87480000</v>
+      </c>
+      <c r="I15" s="45"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="51">
+        <f>F23</f>
+        <v>29160000</v>
+      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="51">
+        <f>B17*1</f>
+        <v>29160000</v>
+      </c>
+      <c r="C18" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="36">
-        <f>F18</f>
-        <v>243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="D18" s="51">
+        <f>B17*4</f>
+        <v>116640000</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="39">
+        <f>B17*3</f>
+        <v>87480000</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="42">
+        <f>B17*1</f>
+        <v>29160000</v>
+      </c>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="42">
+        <f>5/4*B18</f>
+        <v>36450000</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="43">
+        <f>4/4*B18</f>
+        <v>29160000</v>
+      </c>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="51">
+        <f>H18*1</f>
+        <v>29160000</v>
+      </c>
+      <c r="I19" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="52">
+        <f>H18*1</f>
+        <v>29160000</v>
+      </c>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="53"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="47">
+        <f>1*D19</f>
+        <v>29160000</v>
+      </c>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="45">
+        <f>H19*1</f>
+        <v>29160000</v>
+      </c>
+      <c r="I20" s="45"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="51">
+        <f>F28</f>
+        <v>9720000</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="36">
-        <f>B12*1</f>
-        <v>243</v>
-      </c>
-      <c r="C13" s="36" t="s">
+      <c r="B23" s="51">
+        <f>B22*1</f>
+        <v>9720000</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="51">
+        <f>B22*4</f>
+        <v>38880000</v>
+      </c>
+      <c r="E23" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="36">
-        <f>B12*4</f>
-        <v>972</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="36">
-        <f>B12*3</f>
-        <v>729</v>
-      </c>
-      <c r="G13" s="37" t="s">
+      <c r="F23" s="39">
+        <f>B22*3</f>
+        <v>29160000</v>
+      </c>
+      <c r="G23" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="38">
-        <f>B12*1</f>
-        <v>243</v>
-      </c>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="45">
-        <f>H13*1</f>
-        <v>243</v>
-      </c>
-      <c r="I14" s="46" t="s">
+      <c r="H23" s="42">
+        <f>B22*1</f>
+        <v>9720000</v>
+      </c>
+      <c r="I23" s="42"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="42">
+        <f>5/4*B23</f>
+        <v>12150000</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="43">
+        <f>4/4*B23</f>
+        <v>9720000</v>
+      </c>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="51">
+        <f>H23*1</f>
+        <v>9720000</v>
+      </c>
+      <c r="I24" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="47">
-        <f>H13*1</f>
-        <v>243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G15" s="40" t="s">
+      <c r="J24" s="52">
+        <f>H23*1</f>
+        <v>9720000</v>
+      </c>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="53"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="47">
+        <f>1*D24</f>
+        <v>9720000</v>
+      </c>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="41">
-        <f>H14*1</f>
-        <v>243</v>
-      </c>
-      <c r="I15" s="41"/>
-      <c r="J15" s="43"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="36">
-        <f>F23</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="H25" s="45">
+        <f>H24*1</f>
+        <v>9720000</v>
+      </c>
+      <c r="I25" s="45"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="51">
+        <f>F33</f>
+        <v>3240000</v>
+      </c>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="51">
+        <f>B27*1</f>
+        <v>3240000</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="51">
+        <f>B27*4</f>
+        <v>12960000</v>
+      </c>
+      <c r="E28" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="36">
-        <f>B17*1</f>
-        <v>81</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="36">
-        <f>B17*4</f>
-        <v>324</v>
-      </c>
-      <c r="E18" s="36" t="s">
+      <c r="F28" s="39">
+        <f>B27*3</f>
+        <v>9720000</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="42">
+        <f>B27*1</f>
+        <v>3240000</v>
+      </c>
+      <c r="I28" s="42"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="42">
+        <f>5/4*B28</f>
+        <v>4050000</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="43">
+        <f>4/4*B28</f>
+        <v>3240000</v>
+      </c>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" s="51">
+        <f>H28*1</f>
+        <v>3240000</v>
+      </c>
+      <c r="I29" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="52">
+        <f>H28*1</f>
+        <v>3240000</v>
+      </c>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="53"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="47">
+        <f>1*D29</f>
+        <v>3240000</v>
+      </c>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="45">
+        <f>H29*1</f>
+        <v>3240000</v>
+      </c>
+      <c r="I30" s="45"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="51"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="51">
+        <f>F38</f>
+        <v>1080000</v>
+      </c>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="51">
+        <f>B32*1</f>
+        <v>1080000</v>
+      </c>
+      <c r="C33" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="36">
-        <f>B17*3</f>
-        <v>243</v>
-      </c>
-      <c r="G18" s="37" t="s">
+      <c r="D33" s="51">
+        <f>B32*4</f>
+        <v>4320000</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="39">
+        <f>B32*3</f>
+        <v>3240000</v>
+      </c>
+      <c r="G33" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="38">
-        <f>B17*1</f>
-        <v>81</v>
-      </c>
-      <c r="I18" s="38"/>
-      <c r="J18" s="39"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G19" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="45">
-        <f>H18*1</f>
-        <v>81</v>
-      </c>
-      <c r="I19" s="46" t="s">
+      <c r="H33" s="42">
+        <f>B32*1</f>
+        <v>1080000</v>
+      </c>
+      <c r="I33" s="42"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="42">
+        <f>5/4*B33</f>
+        <v>1350000</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="43">
+        <f>4/4*B33</f>
+        <v>1080000</v>
+      </c>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="51">
+        <f>H33*1</f>
+        <v>1080000</v>
+      </c>
+      <c r="I34" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="J19" s="47">
-        <f>H18*1</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="40" t="s">
+      <c r="J34" s="52">
+        <f>H33*1</f>
+        <v>1080000</v>
+      </c>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="53"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="47">
+        <f>1*D34</f>
+        <v>1080000</v>
+      </c>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="41">
-        <f>H19*1</f>
-        <v>81</v>
-      </c>
-      <c r="I20" s="41"/>
-      <c r="J20" s="43"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="36">
-        <f>F28</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="H35" s="45">
+        <f>H34*1</f>
+        <v>1080000</v>
+      </c>
+      <c r="I35" s="45"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39"/>
+      <c r="P35" s="39"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="51"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="39"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="51">
+        <f>B1</f>
+        <v>360000</v>
+      </c>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="36">
-        <f>B22*1</f>
-        <v>27</v>
-      </c>
-      <c r="C23" s="36" t="s">
+      <c r="B38" s="51">
+        <f>B37*1</f>
+        <v>360000</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="51">
+        <f>B37*4</f>
+        <v>1440000</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="39">
+        <f>B37*3</f>
+        <v>1080000</v>
+      </c>
+      <c r="G38" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="42">
+        <f>B37*1</f>
+        <v>360000</v>
+      </c>
+      <c r="I38" s="42"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="42">
+        <f>5/4*B38</f>
+        <v>450000</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="43">
+        <f>4/4*B38</f>
+        <v>360000</v>
+      </c>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="51">
+        <f>H38*1</f>
+        <v>360000</v>
+      </c>
+      <c r="I39" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="36">
-        <f>B22*4</f>
-        <v>108</v>
-      </c>
-      <c r="E23" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="36">
-        <f>B22*3</f>
-        <v>81</v>
-      </c>
-      <c r="G23" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="38">
-        <f>B22*1</f>
-        <v>27</v>
-      </c>
-      <c r="I23" s="38"/>
-      <c r="J23" s="39"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G24" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="45">
-        <f>H23*1</f>
-        <v>27</v>
-      </c>
-      <c r="I24" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="J24" s="47">
-        <f>H23*1</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G25" s="40" t="s">
+      <c r="J39" s="52">
+        <f>H38*1</f>
+        <v>360000</v>
+      </c>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="39"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="53"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="47">
+        <f>1*D39</f>
+        <v>360000</v>
+      </c>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="41">
-        <f>H24*1</f>
-        <v>27</v>
-      </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="43"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="36">
-        <f>F33</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="36">
-        <f>B27*1</f>
-        <v>9</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="36">
-        <f>B27*4</f>
-        <v>36</v>
-      </c>
-      <c r="E28" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="36">
-        <f>B27*3</f>
-        <v>27</v>
-      </c>
-      <c r="G28" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="38">
-        <f>B27*1</f>
-        <v>9</v>
-      </c>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G29" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="45">
-        <f>H28*1</f>
-        <v>9</v>
-      </c>
-      <c r="I29" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="J29" s="47">
-        <f>H28*1</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G30" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" s="41">
-        <f>H29*1</f>
-        <v>9</v>
-      </c>
-      <c r="I30" s="41"/>
-      <c r="J30" s="43"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="36">
-        <f>F38</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="36">
-        <f>B32*1</f>
-        <v>3</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="36">
-        <f>B32*4</f>
-        <v>12</v>
-      </c>
-      <c r="E33" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="F33" s="36">
-        <f>B32*3</f>
-        <v>9</v>
-      </c>
-      <c r="G33" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="H33" s="38">
-        <f>B32*1</f>
-        <v>3</v>
-      </c>
-      <c r="I33" s="38"/>
-      <c r="J33" s="39"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G34" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="H34" s="45">
-        <f>H33*1</f>
-        <v>3</v>
-      </c>
-      <c r="I34" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="J34" s="47">
-        <f>H33*1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G35" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="H35" s="41">
-        <f>H34*1</f>
-        <v>3</v>
-      </c>
-      <c r="I35" s="41"/>
-      <c r="J35" s="43"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="36">
-        <f>B1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="36">
-        <f>B37*1</f>
-        <v>1</v>
-      </c>
-      <c r="C38" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="36">
-        <f>B37*4</f>
-        <v>4</v>
-      </c>
-      <c r="E38" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="36">
-        <f>B37*3</f>
-        <v>3</v>
-      </c>
-      <c r="G38" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="38">
-        <f>B37*1</f>
-        <v>1</v>
-      </c>
-      <c r="I38" s="38"/>
-      <c r="J38" s="39"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G39" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="H39" s="45">
-        <f>H38*1</f>
-        <v>1</v>
-      </c>
-      <c r="I39" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="J39" s="47">
-        <f>H38*1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G40" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="41">
+      <c r="H40" s="45">
         <f>H39*1</f>
-        <v>1</v>
-      </c>
-      <c r="I40" s="41"/>
-      <c r="J40" s="43"/>
+        <v>360000</v>
+      </c>
+      <c r="I40" s="45"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="39"/>
+      <c r="P40" s="39"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="35"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
push 1.4.9b read changelog
</commit_message>
<xml_diff>
--- a/NTC2_-_Compact_Crafting_Recipe_Book.xlsx
+++ b/NTC2_-_Compact_Crafting_Recipe_Book.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MLefebvre\curseforge\minecraft\Instances\1.16.5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10A7B3E-B555-4692-A769-E1E6361BC84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ME Controller" sheetId="2" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="117">
   <si>
     <t>Quantum Ring</t>
   </si>
@@ -310,15 +316,90 @@
   </si>
   <si>
     <t>Redstone Block Per</t>
+  </si>
+  <si>
+    <t>16m wafer</t>
+  </si>
+  <si>
+    <t>1k wafer</t>
+  </si>
+  <si>
+    <t>logic wafer</t>
+  </si>
+  <si>
+    <t>logic processors</t>
+  </si>
+  <si>
+    <t>charged redstone sheet</t>
+  </si>
+  <si>
+    <t>redstone dust</t>
+  </si>
+  <si>
+    <t>charged quartz</t>
+  </si>
+  <si>
+    <t>4k wafer</t>
+  </si>
+  <si>
+    <t>calc wafer</t>
+  </si>
+  <si>
+    <t>calculation processors</t>
+  </si>
+  <si>
+    <t>glassy redstone sheet</t>
+  </si>
+  <si>
+    <t>quartz glass</t>
+  </si>
+  <si>
+    <t>16k wafer</t>
+  </si>
+  <si>
+    <t>64k wafer</t>
+  </si>
+  <si>
+    <t>glowstone dust</t>
+  </si>
+  <si>
+    <t>glassy glowstone sheet</t>
+  </si>
+  <si>
+    <t>256k wafer</t>
+  </si>
+  <si>
+    <t>1m wafer</t>
+  </si>
+  <si>
+    <t>4m wafer</t>
+  </si>
+  <si>
+    <t>redstone</t>
+  </si>
+  <si>
+    <t>logic proc</t>
+  </si>
+  <si>
+    <t>calc proc</t>
+  </si>
+  <si>
+    <t>certus quartz</t>
+  </si>
+  <si>
+    <t>silicon</t>
+  </si>
+  <si>
+    <t>purified certus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
@@ -668,19 +749,19 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
@@ -709,8 +790,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="5" borderId="1" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
@@ -732,13 +813,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="21" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -780,14 +867,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Item"/>
-    <tableColumn id="6" name="EMC/Item"/>
-    <tableColumn id="2" name="Essence per Craft"/>
-    <tableColumn id="3" name="Output per Craft"/>
-    <tableColumn id="4" name="Essence/Item">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="EMC/Item"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Essence per Craft"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Output per Craft"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Essence/Item">
       <calculatedColumnFormula>ROUND(Table1[[#This Row],[Essence per Craft]]/Table1[[#This Row],[Output per Craft]],4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1084,14 +1171,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1112,12 +1199,12 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1207,20 +1294,20 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
+      <c r="A13" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1526,7 +1613,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH30"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -2236,7 +2323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2332,7 +2419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="G1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2346,13 +2433,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="7:11" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
@@ -2434,11 +2521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G9" sqref="G9:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3650,27 +3737,31 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A3:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3864,7 +3955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3874,12 +3965,12 @@
       <c r="C17" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="59">
+      <c r="D17" s="57">
         <f>B18/9</f>
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -3887,6 +3978,876 @@
         <f>B17*9</f>
         <v>36</v>
       </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="37">
+        <f>SUM(D24,F29,F44,F49)+SUM(N30,N35,J24,N40,N45,N50,N55,N60)</f>
+        <v>3456</v>
+      </c>
+      <c r="E20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20">
+        <f>D25</f>
+        <v>288</v>
+      </c>
+      <c r="G20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20">
+        <f>SUM(F30,F35,F40,F45,F50,F55,F60)</f>
+        <v>224</v>
+      </c>
+      <c r="I20" t="s">
+        <v>112</v>
+      </c>
+      <c r="J20">
+        <f>B29</f>
+        <v>288</v>
+      </c>
+      <c r="K20" t="s">
+        <v>113</v>
+      </c>
+      <c r="L20">
+        <f>SUM(B29,B34,B39,B44,B49,B54,B59)</f>
+        <v>2016</v>
+      </c>
+      <c r="M20" t="s">
+        <v>114</v>
+      </c>
+      <c r="N20" s="37">
+        <f>SUM(H30,H35,H40,H45,H50,H55,H60)</f>
+        <v>280</v>
+      </c>
+      <c r="O20" t="s">
+        <v>115</v>
+      </c>
+      <c r="P20" s="37">
+        <f>SUM(L24,L31,L36,L41,L46,L51,L56,L61)</f>
+        <v>2304</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>116</v>
+      </c>
+      <c r="R20" s="37">
+        <f>SUM(L30,L35,L40,L45,L50,L55,L60)</f>
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22">
+        <f>D28</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23">
+        <f>B22*1</f>
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23">
+        <f>B22*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24">
+        <f>B22*9</f>
+        <v>288</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24">
+        <f>D23*9</f>
+        <v>288</v>
+      </c>
+      <c r="G24" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="62">
+        <f>B24*1</f>
+        <v>288</v>
+      </c>
+      <c r="I24" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="62">
+        <f>B24*1</f>
+        <v>288</v>
+      </c>
+      <c r="K24" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="64">
+        <f>B24*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25">
+        <f>D23*9</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27">
+        <f>D33</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28">
+        <f>B27*1</f>
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28">
+        <f>B27*1</f>
+        <v>32</v>
+      </c>
+      <c r="E28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28">
+        <f>B27*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29">
+        <f>B27*9</f>
+        <v>288</v>
+      </c>
+      <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29">
+        <f>F28*9</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30">
+        <f>F28*1</f>
+        <v>32</v>
+      </c>
+      <c r="G30" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="40">
+        <f>5/4*F30</f>
+        <v>40</v>
+      </c>
+      <c r="I30" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="41">
+        <f>4/4*F30</f>
+        <v>32</v>
+      </c>
+      <c r="K30" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="L30" s="40">
+        <f>B29*1</f>
+        <v>288</v>
+      </c>
+      <c r="M30" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N30" s="41">
+        <f>B29*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G31" s="51"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" s="45">
+        <f>1*J30</f>
+        <v>32</v>
+      </c>
+      <c r="K31" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="43">
+        <f>L30*1</f>
+        <v>288</v>
+      </c>
+      <c r="M31" s="43"/>
+      <c r="N31" s="45"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32">
+        <f>D38</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33">
+        <f>B32*1</f>
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33">
+        <f>B32*1</f>
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33">
+        <f>B32*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34">
+        <f>B32*9</f>
+        <v>288</v>
+      </c>
+      <c r="E34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34">
+        <f>F33*4</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35">
+        <f>F33*1</f>
+        <v>32</v>
+      </c>
+      <c r="G35" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" s="40">
+        <f>5/4*F35</f>
+        <v>40</v>
+      </c>
+      <c r="I35" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J35" s="41">
+        <f>4/4*F35</f>
+        <v>32</v>
+      </c>
+      <c r="K35" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="L35" s="40">
+        <f>B34*1</f>
+        <v>288</v>
+      </c>
+      <c r="M35" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N35" s="41">
+        <f>B34*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G36" s="51"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J36" s="45">
+        <f>1*J35</f>
+        <v>32</v>
+      </c>
+      <c r="K36" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="43">
+        <f>L35*1</f>
+        <v>288</v>
+      </c>
+      <c r="M36" s="43"/>
+      <c r="N36" s="45"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37">
+        <f>D43</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38">
+        <f>B37*1</f>
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38">
+        <f>B37*1</f>
+        <v>32</v>
+      </c>
+      <c r="E38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38">
+        <f>B37*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39">
+        <f>B37*9</f>
+        <v>288</v>
+      </c>
+      <c r="E39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39">
+        <f>F38*4</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40">
+        <f>F38*1</f>
+        <v>32</v>
+      </c>
+      <c r="G40" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H40" s="40">
+        <f>5/4*F40</f>
+        <v>40</v>
+      </c>
+      <c r="I40" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J40" s="41">
+        <f>4/4*F40</f>
+        <v>32</v>
+      </c>
+      <c r="K40" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="L40" s="40">
+        <f>B39*1</f>
+        <v>288</v>
+      </c>
+      <c r="M40" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" s="41">
+        <f>B39*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G41" s="51"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J41" s="45">
+        <f>1*J40</f>
+        <v>32</v>
+      </c>
+      <c r="K41" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" s="43">
+        <f>L40*1</f>
+        <v>288</v>
+      </c>
+      <c r="M41" s="43"/>
+      <c r="N41" s="45"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42">
+        <f>D48</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43">
+        <f>B42*1</f>
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43">
+        <f>B42*1</f>
+        <v>32</v>
+      </c>
+      <c r="E43" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43">
+        <f>B42*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44">
+        <f>B42*9</f>
+        <v>288</v>
+      </c>
+      <c r="E44" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44">
+        <f>F43*9</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45">
+        <f>F43*1</f>
+        <v>32</v>
+      </c>
+      <c r="G45" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H45" s="40">
+        <f>5/4*F45</f>
+        <v>40</v>
+      </c>
+      <c r="I45" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J45" s="41">
+        <f>4/4*F45</f>
+        <v>32</v>
+      </c>
+      <c r="K45" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="L45" s="40">
+        <f>B44*1</f>
+        <v>288</v>
+      </c>
+      <c r="M45" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N45" s="41">
+        <f>B44*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G46" s="51"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J46" s="45">
+        <f>1*J45</f>
+        <v>32</v>
+      </c>
+      <c r="K46" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" s="43">
+        <f>L45*1</f>
+        <v>288</v>
+      </c>
+      <c r="M46" s="43"/>
+      <c r="N46" s="45"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47">
+        <f>D53</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48">
+        <f>B47*1</f>
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48">
+        <f>B47*1</f>
+        <v>32</v>
+      </c>
+      <c r="E48" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48">
+        <f>B47*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49">
+        <f>B47*9</f>
+        <v>288</v>
+      </c>
+      <c r="E49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49">
+        <f>F48*9</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>103</v>
+      </c>
+      <c r="F50">
+        <f>F48*1</f>
+        <v>32</v>
+      </c>
+      <c r="G50" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="40">
+        <f>5/4*F50</f>
+        <v>40</v>
+      </c>
+      <c r="I50" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J50" s="41">
+        <f>4/4*F50</f>
+        <v>32</v>
+      </c>
+      <c r="K50" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="L50" s="40">
+        <f>B49*1</f>
+        <v>288</v>
+      </c>
+      <c r="M50" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N50" s="41">
+        <f>B49*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G51" s="51"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J51" s="45">
+        <f>1*J50</f>
+        <v>32</v>
+      </c>
+      <c r="K51" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="43">
+        <f>L50*1</f>
+        <v>288</v>
+      </c>
+      <c r="M51" s="43"/>
+      <c r="N51" s="45"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52">
+        <f>D58</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53">
+        <f>B52*1</f>
+        <v>32</v>
+      </c>
+      <c r="C53" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53">
+        <f>B52*1</f>
+        <v>32</v>
+      </c>
+      <c r="E53" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53">
+        <f>B52*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54">
+        <f>B52*9</f>
+        <v>288</v>
+      </c>
+      <c r="E54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F54">
+        <f>F53*4</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55">
+        <f>F53*1</f>
+        <v>32</v>
+      </c>
+      <c r="G55" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="40">
+        <f>5/4*F55</f>
+        <v>40</v>
+      </c>
+      <c r="I55" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J55" s="41">
+        <f>4/4*F55</f>
+        <v>32</v>
+      </c>
+      <c r="K55" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="L55" s="40">
+        <f>B54*1</f>
+        <v>288</v>
+      </c>
+      <c r="M55" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N55" s="41">
+        <f>B54*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G56" s="51"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J56" s="45">
+        <f>1*J55</f>
+        <v>32</v>
+      </c>
+      <c r="K56" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56" s="43">
+        <f>L55*1</f>
+        <v>288</v>
+      </c>
+      <c r="M56" s="43"/>
+      <c r="N56" s="45"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57">
+        <f>B20</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58">
+        <f>B57*1</f>
+        <v>32</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58">
+        <f>B57*1</f>
+        <v>32</v>
+      </c>
+      <c r="E58" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58">
+        <f>B57*1</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59">
+        <f>B57*9</f>
+        <v>288</v>
+      </c>
+      <c r="E59" t="s">
+        <v>106</v>
+      </c>
+      <c r="F59">
+        <f>F58*4</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>103</v>
+      </c>
+      <c r="F60">
+        <f>F58*1</f>
+        <v>32</v>
+      </c>
+      <c r="G60" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="H60" s="40">
+        <f>5/4*F60</f>
+        <v>40</v>
+      </c>
+      <c r="I60" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J60" s="41">
+        <f>4/4*F60</f>
+        <v>32</v>
+      </c>
+      <c r="K60" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="L60" s="40">
+        <f>B59*1</f>
+        <v>288</v>
+      </c>
+      <c r="M60" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="N60" s="41">
+        <f>B59*1</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G61" s="51"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J61" s="45">
+        <f>1*J60</f>
+        <v>32</v>
+      </c>
+      <c r="K61" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L61" s="43">
+        <f>L60*1</f>
+        <v>288</v>
+      </c>
+      <c r="M61" s="43"/>
+      <c r="N61" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>